<commit_message>
one new test added and changes done in Base.java
</commit_message>
<xml_diff>
--- a/resources/Testdata.xlsx
+++ b/resources/Testdata.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Eclipse\AutomationExercise\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Eclipse2\AutomationExercise\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EDE20D8-7D22-4852-9CC2-4C94BB0B20CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DB06DA9-00DB-4C80-B2CD-F7DAF4458475}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Testdata" sheetId="5" r:id="rId1"/>
+    <sheet name="Cart Testdata" sheetId="6" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="45">
   <si>
     <t>Name</t>
   </si>
@@ -154,6 +155,12 @@
   </si>
   <si>
     <t>Fail</t>
+  </si>
+  <si>
+    <t>TC Name</t>
+  </si>
+  <si>
+    <t>Validate Cart Message</t>
   </si>
 </sst>
 </file>
@@ -485,8 +492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2421FF7-B849-413B-82E4-546BCF9EC3D6}">
   <dimension ref="A1:T4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -741,4 +748,39 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A2EFB0B-357E-482A-B761-BFC825471987}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="20.0"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="13.5703125"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s" s="0">
+        <v>44</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>